<commit_message>
Salesforce Python code and other things.
</commit_message>
<xml_diff>
--- a/Stuff/dow.xlsx
+++ b/Stuff/dow.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F75CB3-A244-4B47-B345-928A998369B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C70C6-17D8-4300-A1A9-AE64B7D02216}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>4K</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>401k</t>
   </si>
@@ -42,13 +39,19 @@
     <t>Vested</t>
   </si>
   <si>
-    <t>otp</t>
-  </si>
-  <si>
-    <t>safar</t>
-  </si>
-  <si>
     <t>Door-sanchar</t>
+  </si>
+  <si>
+    <t>401K</t>
+  </si>
+  <si>
+    <t>Off - 22 days</t>
+  </si>
+  <si>
+    <t>PFS-Web</t>
+  </si>
+  <si>
+    <t>22 days</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360ABBD0-B6F2-4B60-80F9-7AD0E54B9A1D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -389,63 +392,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:F15"/>
+  <dimension ref="C5:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>154</v>
       </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>180</v>
+      </c>
+      <c r="I6">
+        <f>165*0.12</f>
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7">
         <f>(C6*0.06)</f>
         <v>9.24</v>
       </c>
       <c r="D7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f>19*0.12</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="I7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <f>SUM(I6:I7)</f>
+        <v>184.8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10">
         <f>SUM(C6:C9)</f>
         <v>164.24</v>
       </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>SUM(F6:F9)</f>
+        <v>182.28</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
         <v>5</v>
       </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F12" s="1"/>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C15">
         <f>SUM(C10:C14)</f>
-        <v>186.24</v>
+        <v>176.24</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F10:F14)</f>
+        <v>194.28</v>
       </c>
     </row>
   </sheetData>
@@ -466,13 +500,13 @@
   <sheetData>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>